<commit_message>
[updated files with directions]
</commit_message>
<xml_diff>
--- a/DOI list for text classification order.xlsx
+++ b/DOI list for text classification order.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliachotoo/ScrapyArticles/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECE812C-494C-1C45-8A05-72FDEC2EE7B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1048,18 +1049,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1092,17 +1087,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1398,7 +1391,7 @@
   <dimension ref="A1:E313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1403,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="3">
         <v>0</v>
       </c>
       <c r="D1">
@@ -1424,7 +1417,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="D2">
@@ -1438,7 +1431,7 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="D3">
@@ -1449,19 +1442,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
       <c r="E5" s="1"/>
@@ -1470,7 +1463,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
       <c r="E6" s="1"/>
@@ -1479,7 +1472,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>0</v>
       </c>
       <c r="E7" s="1"/>
@@ -1488,16 +1481,16 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
@@ -1506,7 +1499,7 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="1"/>
@@ -1515,16 +1508,16 @@
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="E12" s="1"/>
@@ -1533,61 +1526,61 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0</v>
       </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>0</v>
       </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>0</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>0</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>0</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>1</v>
       </c>
       <c r="C19" t="s">
@@ -1599,19 +1592,19 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="3">
         <v>0</v>
       </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <v>0</v>
       </c>
       <c r="E21" s="1"/>
@@ -1626,55 +1619,55 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="3">
         <v>0</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <v>0</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="3">
         <v>0</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="3">
         <v>0</v>
       </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="3">
         <v>0</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="3">
         <v>0</v>
       </c>
       <c r="E28" s="1"/>
@@ -1689,37 +1682,37 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="3">
         <v>0</v>
       </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="3">
         <v>0</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="3">
         <v>0</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="3">
         <v>2</v>
       </c>
       <c r="E33" s="1"/>
@@ -1734,109 +1727,109 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="3">
         <v>0</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="3">
         <v>0</v>
       </c>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="3">
         <v>0</v>
       </c>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="3">
         <v>2</v>
       </c>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="3">
         <v>0</v>
       </c>
       <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="3">
         <v>2</v>
       </c>
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="3">
         <v>0</v>
       </c>
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="3">
         <v>0</v>
       </c>
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="3">
         <v>0</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="3">
         <v>0</v>
       </c>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="3">
         <v>0</v>
       </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="3">
         <v>0</v>
       </c>
       <c r="E46" s="1"/>
@@ -1860,46 +1853,46 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="3">
         <v>0</v>
       </c>
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="3">
         <v>2</v>
       </c>
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="3">
         <v>0</v>
       </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="3">
         <v>0</v>
       </c>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="3">
         <v>0</v>
       </c>
       <c r="E53" s="1"/>
@@ -1923,7 +1916,7 @@
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="6" t="s">
         <v>286</v>
       </c>
       <c r="B56">
@@ -1941,19 +1934,19 @@
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="3">
         <v>0</v>
       </c>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="3">
         <v>0</v>
       </c>
       <c r="E59" s="1"/>
@@ -1968,19 +1961,19 @@
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="3">
         <v>0</v>
       </c>
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="3">
         <v>1</v>
       </c>
       <c r="C62" t="s">
@@ -1989,64 +1982,64 @@
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="3">
         <v>2</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="3">
         <v>0</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="3">
         <v>2</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="3">
         <v>0</v>
       </c>
       <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="3">
         <v>2</v>
       </c>
       <c r="E67" s="1"/>
     </row>
     <row r="68" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="3">
         <v>0</v>
       </c>
       <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="3">
         <v>0</v>
       </c>
       <c r="E69" s="1"/>
@@ -2061,10 +2054,10 @@
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="3">
         <v>0</v>
       </c>
       <c r="E71" s="1"/>
@@ -2079,46 +2072,46 @@
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="E73" s="1"/>
     </row>
     <row r="74" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="3">
         <v>0</v>
       </c>
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="3">
         <v>2</v>
       </c>
       <c r="E75" s="1"/>
     </row>
     <row r="76" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="3">
         <v>0</v>
       </c>
       <c r="E76" s="1"/>
     </row>
     <row r="77" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="3">
         <v>0</v>
       </c>
       <c r="E77" s="1"/>
@@ -2133,28 +2126,28 @@
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="3">
         <v>0</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="3">
         <v>2</v>
       </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="3">
         <v>1</v>
       </c>
       <c r="C81" t="s">
@@ -2163,28 +2156,28 @@
       <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="3">
         <v>0</v>
       </c>
       <c r="E82" s="1"/>
     </row>
     <row r="83" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="3">
         <v>0</v>
       </c>
       <c r="E83" s="1"/>
     </row>
     <row r="84" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="3">
         <v>0</v>
       </c>
       <c r="C84" t="s">
@@ -2193,190 +2186,190 @@
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="3">
         <v>0</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="3">
         <v>2</v>
       </c>
       <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+      <c r="A87" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="3">
         <v>2</v>
       </c>
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="3">
         <v>0</v>
       </c>
       <c r="E88" s="1"/>
     </row>
     <row r="89" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="3">
         <v>0</v>
       </c>
       <c r="E89" s="1"/>
     </row>
     <row r="90" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="3">
         <v>0</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B91" s="5">
+      <c r="B91" s="3">
         <v>0</v>
       </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="3">
         <v>0</v>
       </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B93" s="5">
+      <c r="B93" s="3">
         <v>0</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="3">
         <v>0</v>
       </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B95" s="5">
+      <c r="B95" s="3">
         <v>0</v>
       </c>
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B96" s="3">
         <v>0</v>
       </c>
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B97" s="3">
         <v>1</v>
       </c>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="3">
         <v>0</v>
       </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="3">
         <v>0</v>
       </c>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B100" s="3">
         <v>0</v>
       </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B101" s="3">
         <v>0</v>
       </c>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B102" s="3">
         <v>0</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B103" s="3">
         <v>0</v>
       </c>
       <c r="E103" s="1"/>
     </row>
     <row r="104" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B104" s="3">
         <v>0</v>
       </c>
       <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B105" s="5">
+      <c r="B105" s="3">
         <v>1</v>
       </c>
       <c r="C105" t="s">
@@ -2385,100 +2378,100 @@
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B106" s="3">
         <v>0</v>
       </c>
       <c r="E106" s="1"/>
     </row>
     <row r="107" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B107" s="5">
+      <c r="B107" s="3">
         <v>0</v>
       </c>
       <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B108" s="3">
         <v>0</v>
       </c>
       <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B109" s="5">
+      <c r="B109" s="3">
         <v>0</v>
       </c>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
+      <c r="A110" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="3">
         <v>2</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B111" s="3">
         <v>1</v>
       </c>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B112" s="3">
         <v>0</v>
       </c>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B113" s="5">
+      <c r="B113" s="3">
         <v>0</v>
       </c>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B114" s="3">
         <v>0</v>
       </c>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B115" s="3">
         <v>0</v>
       </c>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B116" s="3">
         <v>0</v>
       </c>
       <c r="C116" t="s">
@@ -2490,64 +2483,64 @@
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B117" s="3">
         <v>0</v>
       </c>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="3">
         <v>0</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B119" s="3">
         <v>0</v>
       </c>
       <c r="E119" s="1"/>
     </row>
     <row r="120" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="3">
         <v>2</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B121" s="3">
         <v>0</v>
       </c>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
+      <c r="A122" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B122" s="3">
         <v>0</v>
       </c>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A123" s="6" t="s">
+      <c r="A123" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B123" s="7">
+      <c r="B123" s="5">
         <v>2</v>
       </c>
       <c r="C123" t="s">
@@ -2556,19 +2549,19 @@
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B124" s="3">
         <v>0</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B125" s="7">
+      <c r="B125" s="5">
         <v>1</v>
       </c>
       <c r="C125" t="s">
@@ -2577,154 +2570,154 @@
       <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126" s="3">
         <v>0</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="3">
         <v>0</v>
       </c>
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="3">
         <v>0</v>
       </c>
       <c r="E128" s="1"/>
     </row>
     <row r="129" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B129" s="5">
+      <c r="B129" s="3">
         <v>2</v>
       </c>
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A130" s="8" t="s">
+      <c r="A130" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B130" s="5">
+      <c r="B130" s="3">
         <v>2</v>
       </c>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131" s="3">
         <v>0</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B132" s="5">
+      <c r="B132" s="3">
         <v>0</v>
       </c>
       <c r="E132" s="1"/>
     </row>
     <row r="133" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B133" s="5">
+      <c r="B133" s="3">
         <v>0</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A134" s="8" t="s">
+      <c r="A134" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="B134" s="5">
+      <c r="B134" s="3">
         <v>2</v>
       </c>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B135" s="5">
+      <c r="B135" s="3">
         <v>0</v>
       </c>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="3">
         <v>1</v>
       </c>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B137" s="5">
+      <c r="B137" s="3">
         <v>0</v>
       </c>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B138" s="5">
+      <c r="B138" s="3">
         <v>0</v>
       </c>
       <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B139" s="5">
+      <c r="B139" s="3">
         <v>0</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B140" s="7">
+      <c r="B140" s="5">
         <v>0</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B141" s="3">
         <v>0</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142" s="3">
         <v>2</v>
       </c>
       <c r="C142" t="s">
@@ -2733,82 +2726,82 @@
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143" s="3">
         <v>0</v>
       </c>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144" s="3">
         <v>0</v>
       </c>
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B145" s="5">
+      <c r="B145" s="3">
         <v>0</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B146" s="3">
         <v>0</v>
       </c>
       <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B147" s="3">
         <v>2</v>
       </c>
       <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
+      <c r="A148" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B148" s="3">
         <v>2</v>
       </c>
       <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B149" s="3">
         <v>0</v>
       </c>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
+      <c r="A150" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B150" s="3">
         <v>2</v>
       </c>
       <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B151" s="3">
         <v>1</v>
       </c>
       <c r="C151" t="s">
@@ -2817,19 +2810,19 @@
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B152" s="3">
         <v>1</v>
       </c>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B153" s="5">
+      <c r="B153" s="3">
         <v>2</v>
       </c>
       <c r="E153" s="1"/>
@@ -2844,7 +2837,7 @@
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A155" s="8" t="s">
+      <c r="A155" s="6" t="s">
         <v>296</v>
       </c>
       <c r="B155">
@@ -2853,10 +2846,10 @@
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156" s="3">
         <v>1</v>
       </c>
       <c r="C156" t="s">
@@ -2865,145 +2858,145 @@
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
+      <c r="A157" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157" s="3">
         <v>2</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="3">
         <v>0</v>
       </c>
       <c r="E158" s="1"/>
     </row>
     <row r="159" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159" s="3">
         <v>0</v>
       </c>
       <c r="E159" s="1"/>
     </row>
     <row r="160" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B160" s="5">
+      <c r="B160" s="3">
         <v>0</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B161" s="5">
+      <c r="B161" s="3">
         <v>0</v>
       </c>
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B162" s="5">
+      <c r="B162" s="3">
         <v>0</v>
       </c>
       <c r="E162" s="1"/>
     </row>
     <row r="163" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B163" s="5">
+      <c r="B163" s="3">
         <v>0</v>
       </c>
       <c r="E163" s="1"/>
     </row>
     <row r="164" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B164" s="5">
+      <c r="B164" s="3">
         <v>0</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A165" s="8" t="s">
+      <c r="A165" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="B165" s="5">
+      <c r="B165" s="3">
         <v>2</v>
       </c>
       <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B166" s="5">
+      <c r="B166" s="3">
         <v>0</v>
       </c>
       <c r="E166" s="1"/>
     </row>
     <row r="167" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A167" s="8" t="s">
+      <c r="A167" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="B167" s="5">
+      <c r="B167" s="3">
         <v>2</v>
       </c>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B168" s="5">
+      <c r="B168" s="3">
         <v>0</v>
       </c>
       <c r="E168" s="1"/>
     </row>
     <row r="169" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B169" s="5">
+      <c r="B169" s="3">
         <v>0</v>
       </c>
       <c r="E169" s="1"/>
     </row>
     <row r="170" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B170" s="5">
+      <c r="B170" s="3">
         <v>2</v>
       </c>
       <c r="E170" s="1"/>
     </row>
     <row r="171" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A171" s="8" t="s">
+      <c r="A171" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B171" s="5">
+      <c r="B171" s="3">
         <v>2</v>
       </c>
       <c r="E171" s="1"/>
     </row>
     <row r="172" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B172" s="5">
+      <c r="B172" s="3">
         <v>0</v>
       </c>
       <c r="C172" t="s">
@@ -3012,55 +3005,55 @@
       <c r="E172" s="1"/>
     </row>
     <row r="173" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B173" s="5">
+      <c r="B173" s="3">
         <v>0</v>
       </c>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B174" s="5">
+      <c r="B174" s="3">
         <v>0</v>
       </c>
       <c r="E174" s="1"/>
     </row>
     <row r="175" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B175" s="5">
+      <c r="B175" s="3">
         <v>0</v>
       </c>
       <c r="E175" s="1"/>
     </row>
     <row r="176" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
+      <c r="A176" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B176" s="5">
+      <c r="B176" s="3">
         <v>0</v>
       </c>
       <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A177" s="8" t="s">
+      <c r="A177" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="B177" s="5">
+      <c r="B177" s="3">
         <v>2</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A178" s="8" t="s">
+      <c r="A178" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B178" s="5">
+      <c r="B178" s="3">
         <v>2</v>
       </c>
       <c r="E178" s="1"/>
@@ -3075,7 +3068,7 @@
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A180" s="8" t="s">
+      <c r="A180" s="6" t="s">
         <v>303</v>
       </c>
       <c r="B180">
@@ -3084,28 +3077,28 @@
       <c r="E180" s="1"/>
     </row>
     <row r="181" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B181" s="5">
+      <c r="B181" s="3">
         <v>0</v>
       </c>
       <c r="E181" s="1"/>
     </row>
     <row r="182" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A182" s="8" t="s">
+      <c r="A182" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B182" s="5">
+      <c r="B182" s="3">
         <v>2</v>
       </c>
       <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B183" s="5">
+      <c r="B183" s="3">
         <v>1</v>
       </c>
       <c r="C183" t="s">
@@ -3114,19 +3107,19 @@
       <c r="E183" s="1"/>
     </row>
     <row r="184" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B184" s="5">
+      <c r="B184" s="3">
         <v>1</v>
       </c>
       <c r="E184" s="1"/>
     </row>
     <row r="185" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B185" s="5">
+      <c r="B185" s="3">
         <v>1</v>
       </c>
       <c r="C185" t="s">
@@ -3144,28 +3137,28 @@
       <c r="E186" s="1"/>
     </row>
     <row r="187" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B187" s="5">
+      <c r="B187" s="3">
         <v>0</v>
       </c>
       <c r="E187" s="1"/>
     </row>
     <row r="188" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A188" s="8" t="s">
+      <c r="A188" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B188" s="5">
+      <c r="B188" s="3">
         <v>2</v>
       </c>
       <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A189" s="6" t="s">
+      <c r="A189" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B189" s="5">
+      <c r="B189" s="3">
         <v>1</v>
       </c>
       <c r="C189" t="s">
@@ -3174,109 +3167,109 @@
       <c r="E189" s="1"/>
     </row>
     <row r="190" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B190" s="5">
+      <c r="B190" s="3">
         <v>0</v>
       </c>
       <c r="E190" s="1"/>
     </row>
     <row r="191" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
+      <c r="A191" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B191" s="5">
+      <c r="B191" s="3">
         <v>0</v>
       </c>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A192" s="3" t="s">
+      <c r="A192" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B192" s="5">
+      <c r="B192" s="3">
         <v>2</v>
       </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
+      <c r="A193" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B193" s="5">
+      <c r="B193" s="3">
         <v>0</v>
       </c>
       <c r="E193" s="1"/>
     </row>
     <row r="194" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A194" s="3" t="s">
+      <c r="A194" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B194" s="5">
+      <c r="B194" s="3">
         <v>0</v>
       </c>
       <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
+      <c r="A195" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B195" s="5">
+      <c r="B195" s="3">
         <v>0</v>
       </c>
       <c r="E195" s="1"/>
     </row>
     <row r="196" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A196" s="8" t="s">
+      <c r="A196" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B196" s="5">
+      <c r="B196" s="3">
         <v>2</v>
       </c>
       <c r="E196" s="1"/>
     </row>
     <row r="197" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A197" s="3" t="s">
+      <c r="A197" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B197" s="5">
+      <c r="B197" s="3">
         <v>0</v>
       </c>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B198" s="5">
+      <c r="B198" s="3">
         <v>0</v>
       </c>
       <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B199" s="5">
+      <c r="B199" s="3">
         <v>0</v>
       </c>
       <c r="E199" s="1"/>
     </row>
     <row r="200" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A200" s="3" t="s">
+      <c r="A200" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B200" s="5">
+      <c r="B200" s="3">
         <v>0</v>
       </c>
       <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A201" s="3" t="s">
+      <c r="A201" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B201" s="5">
+      <c r="B201" s="3">
         <v>0</v>
       </c>
       <c r="C201" t="s">
@@ -3285,64 +3278,64 @@
       <c r="E201" s="1"/>
     </row>
     <row r="202" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A202" s="3" t="s">
+      <c r="A202" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B202" s="5">
+      <c r="B202" s="3">
         <v>2</v>
       </c>
       <c r="E202" s="1"/>
     </row>
     <row r="203" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A203" s="3" t="s">
+      <c r="A203" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B203" s="5">
+      <c r="B203" s="3">
         <v>0</v>
       </c>
       <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A204" s="8" t="s">
+      <c r="A204" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B204" s="5">
+      <c r="B204" s="3">
         <v>2</v>
       </c>
       <c r="E204" s="1"/>
     </row>
     <row r="205" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
+      <c r="A205" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B205" s="5">
+      <c r="B205" s="3">
         <v>0</v>
       </c>
       <c r="E205" s="1"/>
     </row>
     <row r="206" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A206" s="8" t="s">
+      <c r="A206" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="B206" s="5">
+      <c r="B206" s="3">
         <v>2</v>
       </c>
       <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A207" s="3" t="s">
+      <c r="A207" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B207" s="5">
+      <c r="B207" s="3">
         <v>1</v>
       </c>
       <c r="E207" s="1"/>
     </row>
     <row r="208" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B208" s="5">
+      <c r="B208" s="3">
         <v>1</v>
       </c>
       <c r="C208" t="s">
@@ -3351,155 +3344,155 @@
       <c r="E208" s="1"/>
     </row>
     <row r="209" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A209" s="3" t="s">
+      <c r="A209" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B209" s="5">
+      <c r="B209" s="3">
         <v>0</v>
       </c>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B210" s="5">
+      <c r="B210" s="3">
         <v>0</v>
       </c>
       <c r="E210" s="1"/>
     </row>
     <row r="211" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A211" s="3" t="s">
+      <c r="A211" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B211" s="5">
+      <c r="B211" s="3">
         <v>0</v>
       </c>
       <c r="E211" s="1"/>
     </row>
     <row r="212" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
+      <c r="A212" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B212" s="5">
+      <c r="B212" s="3">
         <v>0</v>
       </c>
       <c r="E212" s="1"/>
     </row>
     <row r="213" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B213" s="5">
+      <c r="B213" s="3">
         <v>0</v>
       </c>
       <c r="E213" s="1"/>
     </row>
     <row r="214" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A214" s="3" t="s">
+      <c r="A214" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B214" s="5">
+      <c r="B214" s="3">
         <v>0</v>
       </c>
       <c r="E214" s="1"/>
     </row>
     <row r="215" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A215" s="8" t="s">
+      <c r="A215" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B215" s="5">
+      <c r="B215" s="3">
         <v>2</v>
       </c>
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B216" s="5">
+      <c r="B216" s="3">
         <v>0</v>
       </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A217" s="3" t="s">
+      <c r="A217" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B217" s="5">
+      <c r="B217" s="3">
         <v>0</v>
       </c>
       <c r="E217" s="1"/>
     </row>
     <row r="218" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A218" s="8" t="s">
+      <c r="A218" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B218" s="5">
+      <c r="B218" s="3">
         <v>2</v>
       </c>
       <c r="E218" s="1"/>
     </row>
     <row r="219" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B219" s="5">
-        <v>0</v>
-      </c>
-      <c r="C219" s="5"/>
+      <c r="B219" s="3">
+        <v>0</v>
+      </c>
+      <c r="C219" s="3"/>
       <c r="E219" s="1"/>
     </row>
     <row r="220" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B220" s="5">
+      <c r="B220" s="3">
         <v>1</v>
       </c>
       <c r="E220" s="1"/>
     </row>
     <row r="221" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A221" s="8" t="s">
+      <c r="A221" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="B221" s="5">
+      <c r="B221" s="3">
         <v>2</v>
       </c>
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A222" s="8" t="s">
+      <c r="A222" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B222" s="5">
+      <c r="B222" s="3">
         <v>2</v>
       </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B223" s="5">
+      <c r="B223" s="3">
         <v>0</v>
       </c>
       <c r="E223" s="1"/>
     </row>
     <row r="224" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A224" s="8" t="s">
+      <c r="A224" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B224" s="5">
+      <c r="B224" s="3">
         <v>2</v>
       </c>
       <c r="E224" s="1"/>
     </row>
     <row r="225" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A225" s="3" t="s">
+      <c r="A225" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B225" s="5">
+      <c r="B225" s="3">
         <v>0</v>
       </c>
       <c r="C225" t="s">
@@ -3508,226 +3501,226 @@
       <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B226" s="5">
+      <c r="B226" s="3">
         <v>0</v>
       </c>
       <c r="E226" s="1"/>
     </row>
     <row r="227" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A227" s="3" t="s">
+      <c r="A227" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B227" s="5">
+      <c r="B227" s="3">
         <v>0</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B228" s="5">
+      <c r="B228" s="3">
         <v>1</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A229" s="3" t="s">
+      <c r="A229" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B229" s="5">
+      <c r="B229" s="3">
         <v>0</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A230" s="3" t="s">
+      <c r="A230" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B230" s="5">
+      <c r="B230" s="3">
         <v>0</v>
       </c>
       <c r="E230" s="1"/>
     </row>
     <row r="231" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A231" s="3" t="s">
+      <c r="A231" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B231" s="5">
+      <c r="B231" s="3">
         <v>0</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A232" s="3" t="s">
+      <c r="A232" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B232" s="5">
+      <c r="B232" s="3">
         <v>0</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A233" s="3" t="s">
+      <c r="A233" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B233" s="5">
+      <c r="B233" s="3">
         <v>0</v>
       </c>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A234" s="3" t="s">
+      <c r="A234" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B234" s="5">
+      <c r="B234" s="3">
         <v>0</v>
       </c>
       <c r="E234" s="1"/>
     </row>
     <row r="235" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A235" s="3" t="s">
+      <c r="A235" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B235" s="5">
+      <c r="B235" s="3">
         <v>0</v>
       </c>
       <c r="E235" s="1"/>
     </row>
     <row r="236" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A236" s="3" t="s">
+      <c r="A236" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B236" s="5">
+      <c r="B236" s="3">
         <v>0</v>
       </c>
       <c r="E236" s="1"/>
     </row>
     <row r="237" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A237" s="3" t="s">
+      <c r="A237" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B237" s="5">
+      <c r="B237" s="3">
         <v>0</v>
       </c>
       <c r="E237" s="1"/>
     </row>
     <row r="238" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A238" s="3" t="s">
+      <c r="A238" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B238" s="5">
+      <c r="B238" s="3">
         <v>0</v>
       </c>
       <c r="E238" s="1"/>
     </row>
     <row r="239" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A239" s="3" t="s">
+      <c r="A239" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B239" s="5">
+      <c r="B239" s="3">
         <v>0</v>
       </c>
       <c r="E239" s="1"/>
     </row>
     <row r="240" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A240" s="8" t="s">
+      <c r="A240" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="B240" s="5">
+      <c r="B240" s="3">
         <v>2</v>
       </c>
       <c r="E240" s="1"/>
     </row>
     <row r="241" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
+      <c r="A241" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B241" s="5">
+      <c r="B241" s="3">
         <v>0</v>
       </c>
       <c r="E241" s="1"/>
     </row>
     <row r="242" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A242" s="3" t="s">
+      <c r="A242" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B242" s="5">
+      <c r="B242" s="3">
         <v>0</v>
       </c>
       <c r="E242" s="1"/>
     </row>
     <row r="243" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A243" s="8" t="s">
+      <c r="A243" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B243" s="5">
+      <c r="B243" s="3">
         <v>2</v>
       </c>
       <c r="E243" s="1"/>
     </row>
     <row r="244" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A244" s="3" t="s">
+      <c r="A244" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B244" s="5">
+      <c r="B244" s="3">
         <v>0</v>
       </c>
       <c r="E244" s="1"/>
     </row>
     <row r="245" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A245" s="3" t="s">
+      <c r="A245" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B245" s="5">
+      <c r="B245" s="3">
         <v>0</v>
       </c>
       <c r="E245" s="1"/>
     </row>
     <row r="246" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B246" s="5">
+      <c r="B246" s="3">
         <v>0</v>
       </c>
       <c r="E246" s="1"/>
     </row>
     <row r="247" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B247" s="5">
+      <c r="B247" s="3">
         <v>0</v>
       </c>
       <c r="E247" s="1"/>
     </row>
     <row r="248" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B248" s="5">
+      <c r="B248" s="3">
         <v>0</v>
       </c>
       <c r="E248" s="1"/>
     </row>
     <row r="249" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A249" s="3" t="s">
+      <c r="A249" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B249" s="5">
+      <c r="B249" s="3">
         <v>0</v>
       </c>
       <c r="E249" s="1"/>
     </row>
     <row r="250" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A250" s="3" t="s">
+      <c r="A250" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B250" s="5">
+      <c r="B250" s="3">
         <v>1</v>
       </c>
       <c r="C250" t="s">
@@ -3736,19 +3729,19 @@
       <c r="E250" s="1"/>
     </row>
     <row r="251" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B251" s="5">
+      <c r="B251" s="3">
         <v>0</v>
       </c>
       <c r="E251" s="1"/>
     </row>
     <row r="252" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A252" s="3" t="s">
+      <c r="A252" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B252" s="5">
+      <c r="B252" s="3">
         <v>1</v>
       </c>
       <c r="C252" t="s">
@@ -3757,10 +3750,10 @@
       <c r="E252" s="1"/>
     </row>
     <row r="253" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A253" s="3" t="s">
+      <c r="A253" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B253" s="5">
+      <c r="B253" s="3">
         <v>1</v>
       </c>
       <c r="C253" t="s">
@@ -3772,523 +3765,523 @@
       <c r="E253" s="1"/>
     </row>
     <row r="254" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A254" s="3" t="s">
+      <c r="A254" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B254" s="5">
+      <c r="B254" s="3">
         <v>0</v>
       </c>
       <c r="E254" s="1"/>
     </row>
     <row r="255" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B255" s="5">
+      <c r="B255" s="3">
         <v>0</v>
       </c>
       <c r="E255" s="1"/>
     </row>
     <row r="256" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A256" s="3" t="s">
+      <c r="A256" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B256" s="5">
+      <c r="B256" s="3">
         <v>0</v>
       </c>
       <c r="E256" s="1"/>
     </row>
     <row r="257" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A257" s="8" t="s">
+      <c r="A257" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="B257" s="5">
+      <c r="B257" s="3">
         <v>2</v>
       </c>
       <c r="E257" s="1"/>
     </row>
     <row r="258" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A258" s="3" t="s">
+      <c r="A258" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B258" s="5">
+      <c r="B258" s="3">
         <v>0</v>
       </c>
       <c r="E258" s="1"/>
     </row>
     <row r="259" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A259" s="3" t="s">
+      <c r="A259" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B259" s="5">
+      <c r="B259" s="3">
         <v>0</v>
       </c>
       <c r="E259" s="1"/>
     </row>
     <row r="260" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A260" s="3" t="s">
+      <c r="A260" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B260" s="5">
+      <c r="B260" s="3">
         <v>0</v>
       </c>
       <c r="E260" s="1"/>
     </row>
     <row r="261" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A261" s="3" t="s">
+      <c r="A261" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B261" s="5">
+      <c r="B261" s="3">
         <v>0</v>
       </c>
       <c r="E261" s="1"/>
     </row>
     <row r="262" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A262" s="3" t="s">
+      <c r="A262" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B262" s="5">
+      <c r="B262" s="3">
         <v>0</v>
       </c>
       <c r="E262" s="1"/>
     </row>
     <row r="263" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A263" s="3" t="s">
+      <c r="A263" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B263" s="5">
+      <c r="B263" s="3">
         <v>0</v>
       </c>
       <c r="E263" s="1"/>
     </row>
     <row r="264" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A264" s="8" t="s">
+      <c r="A264" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B264" s="5">
+      <c r="B264" s="3">
         <v>2</v>
       </c>
       <c r="E264" s="1"/>
     </row>
     <row r="265" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A265" s="8" t="s">
+      <c r="A265" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B265" s="5">
+      <c r="B265" s="3">
         <v>2</v>
       </c>
       <c r="E265" s="1"/>
     </row>
     <row r="266" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A266" s="3" t="s">
+      <c r="A266" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B266" s="5">
+      <c r="B266" s="3">
         <v>0</v>
       </c>
       <c r="E266" s="1"/>
     </row>
     <row r="267" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A267" s="3" t="s">
+      <c r="A267" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B267" s="5">
+      <c r="B267" s="3">
         <v>0</v>
       </c>
       <c r="E267" s="1"/>
     </row>
     <row r="268" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B268" s="5">
+      <c r="B268" s="3">
         <v>1</v>
       </c>
       <c r="E268" s="1"/>
     </row>
     <row r="269" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A269" s="3" t="s">
+      <c r="A269" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B269" s="5">
+      <c r="B269" s="3">
         <v>0</v>
       </c>
       <c r="E269" s="1"/>
     </row>
     <row r="270" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A270" s="3" t="s">
+      <c r="A270" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B270" s="5">
+      <c r="B270" s="3">
         <v>0</v>
       </c>
       <c r="E270" s="1"/>
     </row>
     <row r="271" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A271" s="3" t="s">
+      <c r="A271" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B271" s="5">
+      <c r="B271" s="3">
         <v>0</v>
       </c>
       <c r="E271" s="1"/>
     </row>
     <row r="272" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A272" s="3" t="s">
+      <c r="A272" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B272" s="5">
+      <c r="B272" s="3">
         <v>0</v>
       </c>
       <c r="E272" s="1"/>
     </row>
     <row r="273" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A273" s="8" t="s">
+      <c r="A273" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B273" s="5">
+      <c r="B273" s="3">
         <v>2</v>
       </c>
       <c r="E273" s="1"/>
     </row>
     <row r="274" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A274" s="3" t="s">
+      <c r="A274" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B274" s="5">
+      <c r="B274" s="3">
         <v>0</v>
       </c>
       <c r="E274" s="1"/>
     </row>
     <row r="275" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A275" s="3" t="s">
+      <c r="A275" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B275" s="5">
+      <c r="B275" s="3">
         <v>0</v>
       </c>
       <c r="E275" s="1"/>
     </row>
     <row r="276" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A276" s="3" t="s">
+      <c r="A276" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B276" s="5">
+      <c r="B276" s="3">
         <v>0</v>
       </c>
       <c r="E276" s="1"/>
     </row>
     <row r="277" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A277" s="8" t="s">
+      <c r="A277" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="B277" s="5">
+      <c r="B277" s="3">
         <v>2</v>
       </c>
       <c r="E277" s="1"/>
     </row>
     <row r="278" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A278" s="3" t="s">
+      <c r="A278" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B278" s="5">
+      <c r="B278" s="3">
         <v>1</v>
       </c>
       <c r="E278" s="1"/>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" s="5" t="s">
+      <c r="A279" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B279" s="5">
-        <v>0</v>
-      </c>
-      <c r="E279" s="5"/>
+      <c r="B279" s="3">
+        <v>0</v>
+      </c>
+      <c r="E279" s="3"/>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A280" s="5" t="s">
+      <c r="A280" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B280" s="5">
-        <v>2</v>
-      </c>
-      <c r="E280" s="5"/>
+      <c r="B280" s="3">
+        <v>2</v>
+      </c>
+      <c r="E280" s="3"/>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A281" s="5" t="s">
+      <c r="A281" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B281" s="5">
-        <v>0</v>
-      </c>
-      <c r="E281" s="5"/>
+      <c r="B281" s="3">
+        <v>0</v>
+      </c>
+      <c r="E281" s="3"/>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A282" s="5" t="s">
+      <c r="A282" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B282" s="5">
-        <v>0</v>
-      </c>
-      <c r="E282" s="5"/>
+      <c r="B282" s="3">
+        <v>0</v>
+      </c>
+      <c r="E282" s="3"/>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" s="5" t="s">
+      <c r="A283" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B283" s="5">
-        <v>0</v>
-      </c>
-      <c r="E283" s="5"/>
+      <c r="B283" s="3">
+        <v>0</v>
+      </c>
+      <c r="E283" s="3"/>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" s="5" t="s">
+      <c r="A284" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B284" s="5">
-        <v>0</v>
-      </c>
-      <c r="E284" s="5"/>
+      <c r="B284" s="3">
+        <v>0</v>
+      </c>
+      <c r="E284" s="3"/>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A285" s="5" t="s">
+      <c r="A285" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B285" s="5">
+      <c r="B285" s="3">
         <v>1</v>
       </c>
       <c r="C285" t="s">
         <v>277</v>
       </c>
-      <c r="E285" s="5"/>
+      <c r="E285" s="3"/>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A286" s="5" t="s">
+      <c r="A286" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B286" s="5">
-        <v>0</v>
-      </c>
-      <c r="E286" s="5"/>
+      <c r="B286" s="3">
+        <v>0</v>
+      </c>
+      <c r="E286" s="3"/>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" s="9" t="s">
+      <c r="A287" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="B287" s="5">
-        <v>2</v>
-      </c>
-      <c r="E287" s="5"/>
+      <c r="B287" s="3">
+        <v>2</v>
+      </c>
+      <c r="E287" s="3"/>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="5" t="s">
+      <c r="A288" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B288" s="5">
-        <v>0</v>
-      </c>
-      <c r="E288" s="5"/>
+      <c r="B288" s="3">
+        <v>0</v>
+      </c>
+      <c r="E288" s="3"/>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A289" s="5" t="s">
+      <c r="A289" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B289" s="5">
-        <v>0</v>
-      </c>
-      <c r="E289" s="5"/>
+      <c r="B289" s="3">
+        <v>0</v>
+      </c>
+      <c r="E289" s="3"/>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>245</v>
       </c>
-      <c r="B290" s="5">
-        <v>1</v>
-      </c>
-      <c r="E290" s="5"/>
+      <c r="B290" s="3">
+        <v>1</v>
+      </c>
+      <c r="E290" s="3"/>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A291" s="5" t="s">
+      <c r="A291" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B291" s="5">
-        <v>0</v>
-      </c>
-      <c r="E291" s="5"/>
+      <c r="B291" s="3">
+        <v>0</v>
+      </c>
+      <c r="E291" s="3"/>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" s="5" t="s">
+      <c r="A292" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B292" s="5">
-        <v>0</v>
-      </c>
-      <c r="E292" s="5"/>
+      <c r="B292" s="3">
+        <v>0</v>
+      </c>
+      <c r="E292" s="3"/>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A293" s="5" t="s">
+      <c r="A293" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B293" s="5">
-        <v>0</v>
-      </c>
-      <c r="E293" s="5"/>
+      <c r="B293" s="3">
+        <v>0</v>
+      </c>
+      <c r="E293" s="3"/>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A294" s="5" t="s">
+      <c r="A294" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B294" s="5">
-        <v>1</v>
-      </c>
-      <c r="E294" s="5"/>
+      <c r="B294" s="3">
+        <v>1</v>
+      </c>
+      <c r="E294" s="3"/>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" s="5" t="s">
+      <c r="A295" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B295" s="5">
-        <v>1</v>
-      </c>
-      <c r="E295" s="5"/>
+      <c r="B295" s="3">
+        <v>1</v>
+      </c>
+      <c r="E295" s="3"/>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" s="5" t="s">
+      <c r="A296" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B296" s="5">
-        <v>2</v>
-      </c>
-      <c r="E296" s="5"/>
+      <c r="B296" s="3">
+        <v>2</v>
+      </c>
+      <c r="E296" s="3"/>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>252</v>
       </c>
-      <c r="B297" s="5">
-        <v>1</v>
-      </c>
-      <c r="E297" s="5"/>
+      <c r="B297" s="3">
+        <v>1</v>
+      </c>
+      <c r="E297" s="3"/>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" s="5" t="s">
+      <c r="A298" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B298" s="5">
-        <v>0</v>
-      </c>
-      <c r="E298" s="5"/>
+      <c r="B298" s="3">
+        <v>0</v>
+      </c>
+      <c r="E298" s="3"/>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A299" s="5" t="s">
+      <c r="A299" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B299" s="5">
-        <v>0</v>
-      </c>
-      <c r="E299" s="5"/>
+      <c r="B299" s="3">
+        <v>0</v>
+      </c>
+      <c r="E299" s="3"/>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" s="5" t="s">
+      <c r="A300" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B300" s="5">
-        <v>0</v>
-      </c>
-      <c r="E300" s="5"/>
+      <c r="B300" s="3">
+        <v>0</v>
+      </c>
+      <c r="E300" s="3"/>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A301" s="9" t="s">
+      <c r="A301" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="B301" s="5">
-        <v>2</v>
-      </c>
-      <c r="E301" s="5"/>
+      <c r="B301" s="3">
+        <v>2</v>
+      </c>
+      <c r="E301" s="3"/>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" s="5" t="s">
+      <c r="A302" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B302" s="5">
-        <v>0</v>
-      </c>
-      <c r="E302" s="5"/>
+      <c r="B302" s="3">
+        <v>0</v>
+      </c>
+      <c r="E302" s="3"/>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A303" s="5" t="s">
+      <c r="A303" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B303" s="5">
-        <v>0</v>
-      </c>
-      <c r="E303" s="5"/>
+      <c r="B303" s="3">
+        <v>0</v>
+      </c>
+      <c r="E303" s="3"/>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A304" s="9" t="s">
+      <c r="A304" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B304" s="5">
-        <v>2</v>
-      </c>
-      <c r="E304" s="5"/>
+      <c r="B304" s="3">
+        <v>2</v>
+      </c>
+      <c r="E304" s="3"/>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A305" s="5" t="s">
+      <c r="A305" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B305" s="5">
-        <v>2</v>
-      </c>
-      <c r="E305" s="5"/>
+      <c r="B305" s="3">
+        <v>2</v>
+      </c>
+      <c r="E305" s="3"/>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A306" s="5" t="s">
+      <c r="A306" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B306" s="5">
+      <c r="B306" s="3">
         <v>1</v>
       </c>
       <c r="C306" t="s">
         <v>277</v>
       </c>
-      <c r="E306" s="5"/>
+      <c r="E306" s="3"/>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A307" s="5" t="s">
+      <c r="A307" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B307" s="5">
-        <v>0</v>
-      </c>
-      <c r="E307" s="5"/>
+      <c r="B307" s="3">
+        <v>0</v>
+      </c>
+      <c r="E307" s="3"/>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A308" s="5" t="s">
+      <c r="A308" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B308" s="5">
-        <v>0</v>
-      </c>
-      <c r="E308" s="5"/>
+      <c r="B308" s="3">
+        <v>0</v>
+      </c>
+      <c r="E308" s="3"/>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A309" s="5" t="s">
+      <c r="A309" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B309" s="5">
-        <v>2</v>
-      </c>
-      <c r="E309" s="5"/>
+      <c r="B309" s="3">
+        <v>2</v>
+      </c>
+      <c r="E309" s="3"/>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A310" s="5" t="s">
+      <c r="A310" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B310" s="5">
-        <v>0</v>
-      </c>
-      <c r="E310" s="5"/>
+      <c r="B310" s="3">
+        <v>0</v>
+      </c>
+      <c r="E310" s="3"/>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
@@ -4297,25 +4290,25 @@
       <c r="B311">
         <v>1</v>
       </c>
-      <c r="E311" s="5"/>
+      <c r="E311" s="3"/>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A312" s="5" t="s">
+      <c r="A312" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B312" s="5">
-        <v>0</v>
-      </c>
-      <c r="E312" s="5"/>
+      <c r="B312" s="3">
+        <v>0</v>
+      </c>
+      <c r="E312" s="3"/>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A313" s="5" t="s">
+      <c r="A313" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B313" s="5">
-        <v>0</v>
-      </c>
-      <c r="E313" s="5"/>
+      <c r="B313" s="3">
+        <v>0</v>
+      </c>
+      <c r="E313" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>